<commit_message>
Device IO - Router
</commit_message>
<xml_diff>
--- a/Device IO.xlsx
+++ b/Device IO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28730" windowHeight="17570" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="17565"/>
   </bookViews>
   <sheets>
     <sheet name="Router" sheetId="9" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
   <si>
     <t>Input</t>
   </si>
@@ -120,6 +120,213 @@
   </si>
   <si>
     <t>VDA 01 (4K-SDI PGM)</t>
+  </si>
+  <si>
+    <t>Cam 01 SDI O/P</t>
+  </si>
+  <si>
+    <t>Cam 02 SDI O/P</t>
+  </si>
+  <si>
+    <t>Cam 03 SDI O/P</t>
+  </si>
+  <si>
+    <t>Cam 04 SDI O/P</t>
+  </si>
+  <si>
+    <t>Cam 05 SDI O/P</t>
+  </si>
+  <si>
+    <t>Studio B06</t>
+  </si>
+  <si>
+    <t>Studio B07</t>
+  </si>
+  <si>
+    <t>Studio B08</t>
+  </si>
+  <si>
+    <t>VTR 01 SDI O/P</t>
+  </si>
+  <si>
+    <t>VTR 01 Mon O/P</t>
+  </si>
+  <si>
+    <t>VTR 02 SDI O/P</t>
+  </si>
+  <si>
+    <t>VTR 02 Mon O/P</t>
+  </si>
+  <si>
+    <t>VTR 03 SDI O/P</t>
+  </si>
+  <si>
+    <t>VTR 04 SDI O/P</t>
+  </si>
+  <si>
+    <t>CG 01 Key O/P</t>
+  </si>
+  <si>
+    <t>CG 01 Fill O/P</t>
+  </si>
+  <si>
+    <t>UpCon 01 SDI O/P</t>
+  </si>
+  <si>
+    <t>Embedder 01 SDI O/P</t>
+  </si>
+  <si>
+    <t>Embedder 02 SDI O/P</t>
+  </si>
+  <si>
+    <t>VMX PGM SD O/P</t>
+  </si>
+  <si>
+    <t>VMX ME1 PVW O/P</t>
+  </si>
+  <si>
+    <t>VMX Multiviewer 01 O/P</t>
+  </si>
+  <si>
+    <t>VMX Multiviewer 02 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 01 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 02 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 03 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 04 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 05 O/P</t>
+  </si>
+  <si>
+    <t>VMX Aux 06 O/P</t>
+  </si>
+  <si>
+    <t>CCU Mon 01</t>
+  </si>
+  <si>
+    <t>CCU Mon 03</t>
+  </si>
+  <si>
+    <t>CCU Mon 04</t>
+  </si>
+  <si>
+    <t>CCU Mon 05</t>
+  </si>
+  <si>
+    <t>CCU Mon 06</t>
+  </si>
+  <si>
+    <t>CCU Mon 07</t>
+  </si>
+  <si>
+    <t>VTR Mon 01</t>
+  </si>
+  <si>
+    <t>VTR Mon 02</t>
+  </si>
+  <si>
+    <t>VTR Mon 03</t>
+  </si>
+  <si>
+    <t>VTR Mon 04</t>
+  </si>
+  <si>
+    <t>VTR Audio Mon</t>
+  </si>
+  <si>
+    <t>ACR Mon 01</t>
+  </si>
+  <si>
+    <t>ACR Mon 02</t>
+  </si>
+  <si>
+    <t>ACR Mon 03</t>
+  </si>
+  <si>
+    <t>DeEmbedder 01</t>
+  </si>
+  <si>
+    <t>DeEmbedder 02</t>
+  </si>
+  <si>
+    <t>VTR 01 SDI I/P</t>
+  </si>
+  <si>
+    <t>VTR 02 SDI I/P</t>
+  </si>
+  <si>
+    <t>VTR 03 SDI I/P</t>
+  </si>
+  <si>
+    <t>VTR 04 SDI I/P</t>
+  </si>
+  <si>
+    <t>CG 01 SDI I/P</t>
+  </si>
+  <si>
+    <t>Studio A06</t>
+  </si>
+  <si>
+    <t>Studio A07</t>
+  </si>
+  <si>
+    <t>VMX I/P 1</t>
+  </si>
+  <si>
+    <t>VMX I/P 2</t>
+  </si>
+  <si>
+    <t>VMX I/P 3</t>
+  </si>
+  <si>
+    <t>VMX I/P 4</t>
+  </si>
+  <si>
+    <t>VMX I/P 5</t>
+  </si>
+  <si>
+    <t>VMX I/P 6</t>
+  </si>
+  <si>
+    <t>VMX I/P 7</t>
+  </si>
+  <si>
+    <t>VMX I/P 8</t>
+  </si>
+  <si>
+    <t>VMX I/P 9</t>
+  </si>
+  <si>
+    <t>VMX I/P 10</t>
+  </si>
+  <si>
+    <t>VMX I/P 11</t>
+  </si>
+  <si>
+    <t>VMX I/P 12</t>
+  </si>
+  <si>
+    <t>VMX I/P 13</t>
+  </si>
+  <si>
+    <t>VMX I/P 14</t>
+  </si>
+  <si>
+    <t>VMX I/P 15</t>
+  </si>
+  <si>
+    <t>SDI-HDMI 01 I/P</t>
+  </si>
+  <si>
+    <t>SDI-HDMI 02 I/P</t>
   </si>
 </sst>
 </file>
@@ -157,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -174,11 +381,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -196,6 +427,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,17 +737,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="2" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,6 +762,7 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="9"/>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
@@ -532,330 +773,780 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2001</v>
+      </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2002</v>
+      </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2003</v>
+      </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2004</v>
+      </c>
       <c r="E7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2005</v>
+      </c>
       <c r="E8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2006</v>
+      </c>
       <c r="E9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2007</v>
+      </c>
       <c r="E10" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2008</v>
+      </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2009</v>
+      </c>
       <c r="E12" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2010</v>
+      </c>
       <c r="E13" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2011</v>
+      </c>
       <c r="E14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2012</v>
+      </c>
       <c r="E15" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2013</v>
+      </c>
       <c r="E16" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2014</v>
+      </c>
       <c r="E17" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2015</v>
+      </c>
       <c r="E18" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2016</v>
+      </c>
       <c r="E19" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2017</v>
+      </c>
       <c r="E20" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
+      <c r="C21" s="1">
+        <v>2018</v>
+      </c>
       <c r="E21" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
+      <c r="C22" s="1">
+        <v>2019</v>
+      </c>
       <c r="E22" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
+      <c r="C23" s="1">
+        <v>2020</v>
+      </c>
       <c r="E23" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
+      <c r="C24" s="1">
+        <v>2021</v>
+      </c>
       <c r="E24" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
+      <c r="C25" s="1">
+        <v>2022</v>
+      </c>
       <c r="E25" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
+      <c r="C26" s="1">
+        <v>2023</v>
+      </c>
       <c r="E26" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
+      <c r="C27" s="1">
+        <v>2024</v>
+      </c>
       <c r="E27" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
+      <c r="C28" s="1">
+        <v>2025</v>
+      </c>
       <c r="E28" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
+      <c r="C29" s="1">
+        <v>2026</v>
+      </c>
       <c r="E29" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
+      <c r="C30" s="1">
+        <v>2027</v>
+      </c>
       <c r="E30" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
+      <c r="C31" s="1">
+        <v>2028</v>
+      </c>
       <c r="E31" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2029</v>
+      </c>
       <c r="E32" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>30</v>
       </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2030</v>
+      </c>
       <c r="E33" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31</v>
       </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2031</v>
+      </c>
       <c r="E34" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32</v>
       </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2032</v>
+      </c>
       <c r="E35" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>33</v>
       </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2033</v>
+      </c>
       <c r="E36" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>34</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2034</v>
+      </c>
       <c r="E37" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35</v>
       </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2035</v>
+      </c>
       <c r="E38" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>36</v>
       </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2036</v>
+      </c>
       <c r="E39" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37</v>
       </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2037</v>
+      </c>
       <c r="E40" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38</v>
       </c>
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2038</v>
+      </c>
       <c r="E41" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>39</v>
       </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2039</v>
+      </c>
       <c r="E42" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40</v>
       </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2040</v>
+      </c>
       <c r="E43" s="1">
         <v>40</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2140</v>
       </c>
     </row>
   </sheetData>
@@ -873,14 +1564,14 @@
       <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="11.26953125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -900,13 +1591,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -914,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -922,7 +1613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -930,7 +1621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -938,7 +1629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -946,7 +1637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -954,7 +1645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -962,7 +1653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -970,7 +1661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -978,7 +1669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -986,7 +1677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -994,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1002,42 +1693,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1057,14 +1748,14 @@
       <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="8.7109375" style="4"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1084,16 +1775,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1101,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1109,7 +1800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1117,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1125,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1133,7 +1824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1141,7 +1832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1149,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1157,7 +1848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1165,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1173,7 +1864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1181,7 +1872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1189,7 +1880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1197,7 +1888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1205,7 +1896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1213,7 +1904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1221,7 +1912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1229,7 +1920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1237,7 +1928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1245,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1253,7 +1944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1261,7 +1952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1269,7 +1960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1277,7 +1968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1285,72 +1976,72 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
@@ -1370,12 +2061,12 @@
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1386,58 +2077,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1452,17 +2143,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1482,13 +2173,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1496,48 +2187,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1545,52 +2236,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1598,37 +2289,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1636,42 +2327,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E37" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E38" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E39" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E40" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E42" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E43" s="4" t="s">
         <v>15</v>
       </c>
@@ -1691,12 +2382,12 @@
       <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1707,263 +2398,263 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>8</v>
       </c>

</xml_diff>